<commit_message>
Refactor roll into separate function
</commit_message>
<xml_diff>
--- a/mtg_firmware/timer.xlsx
+++ b/mtg_firmware/timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmp\Documents\Max\mtg_life_counter\mtg_firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F101F22-D64E-4716-BA89-234A6AE83616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
+    <workbookView xWindow="11160" yWindow="3495" windowWidth="14580" windowHeight="9975" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -295,30 +295,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <f>200*8</f>
+        <f>160*10</f>
         <v>1600</v>
       </c>
       <c r="C1" t="s">
@@ -709,91 +709,91 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="18"/>
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="13">
         <v>0</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <f>$B$2/($B$1)-1</f>
         <v>9999</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <f>$B$2/($B$1)-1</f>
         <v>9999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="13">
         <v>8</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <f t="shared" ref="B7:B11" si="0">$B$2/($B$1*A7)-1</f>
         <v>1249</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f>$B$2/($B$1*A7)-1</f>
         <v>1249</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="13">
         <v>32</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="4">
+      <c r="B8" s="11"/>
+      <c r="C8" s="3">
         <f>$B$2/($B$1*A8)-1</f>
         <v>311.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="13">
         <v>64</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="10">
         <f t="shared" si="0"/>
         <v>155.25</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f t="shared" ref="C9" si="1">$B$2/($B$1*A9)-1</f>
         <v>155.25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="13">
         <v>256</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <f t="shared" si="0"/>
         <v>38.0625</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
+      <c r="A11" s="14">
         <v>1024</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <f t="shared" si="0"/>
         <v>8.765625</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Mess w timer excel
</commit_message>
<xml_diff>
--- a/mtg_firmware/timer.xlsx
+++ b/mtg_firmware/timer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmp\Documents\Max\mtg_life_counter\mtg_firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/915f7bc53e120788/Projects/Magic/mtg_life_counter/mtg_firmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26681DC7-75D6-44DF-AE01-FE3806806517}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="3495" windowWidth="14580" windowHeight="9975" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
+    <workbookView xWindow="9750" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,8 +689,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <f>160*10</f>
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -732,11 +731,11 @@
       </c>
       <c r="B6" s="9">
         <f>$B$2/($B$1)-1</f>
-        <v>9999</v>
+        <v>15999</v>
       </c>
       <c r="C6" s="7">
         <f>$B$2/($B$1)-1</f>
-        <v>9999</v>
+        <v>15999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,11 +744,11 @@
       </c>
       <c r="B7" s="10">
         <f t="shared" ref="B7:B11" si="0">$B$2/($B$1*A7)-1</f>
-        <v>1249</v>
+        <v>1999</v>
       </c>
       <c r="C7" s="3">
         <f>$B$2/($B$1*A7)-1</f>
-        <v>1249</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,7 +758,7 @@
       <c r="B8" s="11"/>
       <c r="C8" s="3">
         <f>$B$2/($B$1*A8)-1</f>
-        <v>311.5</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,11 +767,11 @@
       </c>
       <c r="B9" s="10">
         <f t="shared" si="0"/>
-        <v>155.25</v>
+        <v>249</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9" si="1">$B$2/($B$1*A9)-1</f>
-        <v>155.25</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,7 +780,7 @@
       </c>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
-        <v>38.0625</v>
+        <v>61.5</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -791,7 +790,7 @@
       </c>
       <c r="B11" s="12">
         <f t="shared" si="0"/>
-        <v>8.765625</v>
+        <v>14.625</v>
       </c>
       <c r="C11" s="5"/>
     </row>

</xml_diff>

<commit_message>
Copy firmware changes from master
</commit_message>
<xml_diff>
--- a/mtg_firmware/timer.xlsx
+++ b/mtg_firmware/timer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/915f7bc53e120788/Projects/Magic/mtg_life_counter/mtg_firmware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmp\Documents\Max\mtg_life_counter\mtg_firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{26681DC7-75D6-44DF-AE01-FE3806806517}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9750" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
+    <workbookView xWindow="11160" yWindow="3495" windowWidth="14580" windowHeight="9975" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,8 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>1000</v>
+        <f>160*10</f>
+        <v>1600</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -731,11 +732,11 @@
       </c>
       <c r="B6" s="9">
         <f>$B$2/($B$1)-1</f>
-        <v>15999</v>
+        <v>9999</v>
       </c>
       <c r="C6" s="7">
         <f>$B$2/($B$1)-1</f>
-        <v>15999</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,11 +745,11 @@
       </c>
       <c r="B7" s="10">
         <f t="shared" ref="B7:B11" si="0">$B$2/($B$1*A7)-1</f>
-        <v>1999</v>
+        <v>1249</v>
       </c>
       <c r="C7" s="3">
         <f>$B$2/($B$1*A7)-1</f>
-        <v>1999</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,7 +759,7 @@
       <c r="B8" s="11"/>
       <c r="C8" s="3">
         <f>$B$2/($B$1*A8)-1</f>
-        <v>499</v>
+        <v>311.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,11 +768,11 @@
       </c>
       <c r="B9" s="10">
         <f t="shared" si="0"/>
-        <v>249</v>
+        <v>155.25</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9" si="1">$B$2/($B$1*A9)-1</f>
-        <v>249</v>
+        <v>155.25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,7 +781,7 @@
       </c>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
-        <v>61.5</v>
+        <v>38.0625</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -790,7 +791,7 @@
       </c>
       <c r="B11" s="12">
         <f t="shared" si="0"/>
-        <v>14.625</v>
+        <v>8.765625</v>
       </c>
       <c r="C11" s="5"/>
     </row>

</xml_diff>

<commit_message>
Start to remove old software implementation
</commit_message>
<xml_diff>
--- a/mtg_firmware/timer.xlsx
+++ b/mtg_firmware/timer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmp\Documents\Max\mtg_life_counter\mtg_firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/915f7bc53e120788/Projects/Magic/Life Counter/mtg_life_counter/mtg_firmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBAC7DCE-755E-4E84-A665-E57FB626E11E}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="3495" windowWidth="14580" windowHeight="9975" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
+    <workbookView xWindow="-18120" yWindow="-120" windowWidth="18240" windowHeight="23640" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,8 +689,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <f>160*10</f>
-        <v>1600</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -732,11 +731,11 @@
       </c>
       <c r="B6" s="9">
         <f>$B$2/($B$1)-1</f>
-        <v>9999</v>
+        <v>39999</v>
       </c>
       <c r="C6" s="7">
         <f>$B$2/($B$1)-1</f>
-        <v>9999</v>
+        <v>39999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,11 +744,11 @@
       </c>
       <c r="B7" s="10">
         <f t="shared" ref="B7:B11" si="0">$B$2/($B$1*A7)-1</f>
-        <v>1249</v>
+        <v>4999</v>
       </c>
       <c r="C7" s="3">
         <f>$B$2/($B$1*A7)-1</f>
-        <v>1249</v>
+        <v>4999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,7 +758,7 @@
       <c r="B8" s="11"/>
       <c r="C8" s="3">
         <f>$B$2/($B$1*A8)-1</f>
-        <v>311.5</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,11 +767,11 @@
       </c>
       <c r="B9" s="10">
         <f t="shared" si="0"/>
-        <v>155.25</v>
+        <v>624</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9" si="1">$B$2/($B$1*A9)-1</f>
-        <v>155.25</v>
+        <v>624</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,7 +780,7 @@
       </c>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
-        <v>38.0625</v>
+        <v>155.25</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -791,7 +790,7 @@
       </c>
       <c r="B11" s="12">
         <f t="shared" si="0"/>
-        <v>8.765625</v>
+        <v>38.0625</v>
       </c>
       <c r="C11" s="5"/>
     </row>

</xml_diff>

<commit_message>
Get display test working
</commit_message>
<xml_diff>
--- a/mtg_firmware/timer.xlsx
+++ b/mtg_firmware/timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/915f7bc53e120788/Projects/Magic/Life Counter/mtg_life_counter/mtg_firmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBAC7DCE-755E-4E84-A665-E57FB626E11E}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2426D44-4E88-4D69-B5D3-1E8211CCE458}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="-120" windowWidth="18240" windowHeight="23640" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
+    <workbookView xWindow="4425" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>400</v>
+        <v>6400</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -731,11 +731,11 @@
       </c>
       <c r="B6" s="9">
         <f>$B$2/($B$1)-1</f>
-        <v>39999</v>
+        <v>2499</v>
       </c>
       <c r="C6" s="7">
         <f>$B$2/($B$1)-1</f>
-        <v>39999</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,11 +744,11 @@
       </c>
       <c r="B7" s="10">
         <f t="shared" ref="B7:B11" si="0">$B$2/($B$1*A7)-1</f>
-        <v>4999</v>
+        <v>311.5</v>
       </c>
       <c r="C7" s="3">
         <f>$B$2/($B$1*A7)-1</f>
-        <v>4999</v>
+        <v>311.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,7 +758,7 @@
       <c r="B8" s="11"/>
       <c r="C8" s="3">
         <f>$B$2/($B$1*A8)-1</f>
-        <v>1249</v>
+        <v>77.125</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,11 +767,11 @@
       </c>
       <c r="B9" s="10">
         <f t="shared" si="0"/>
-        <v>624</v>
+        <v>38.0625</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9" si="1">$B$2/($B$1*A9)-1</f>
-        <v>624</v>
+        <v>38.0625</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
       </c>
       <c r="B10" s="10">
         <f t="shared" si="0"/>
-        <v>155.25</v>
+        <v>8.765625</v>
       </c>
       <c r="C10" s="4"/>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="B11" s="12">
         <f t="shared" si="0"/>
-        <v>38.0625</v>
+        <v>1.44140625</v>
       </c>
       <c r="C11" s="5"/>
     </row>

</xml_diff>

<commit_message>
Get basic functionality working
</commit_message>
<xml_diff>
--- a/mtg_firmware/timer.xlsx
+++ b/mtg_firmware/timer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/915f7bc53e120788/Projects/Magic/Life Counter/mtg_life_counter/mtg_firmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2426D44-4E88-4D69-B5D3-1E8211CCE458}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{763229F5-79F4-4157-8ACD-E478CBD5690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9DFD007-E5D9-4F81-AEDD-843E39CEC826}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="2745" windowWidth="21600" windowHeight="11385" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
+    <workbookView xWindow="15855" yWindow="2235" windowWidth="21600" windowHeight="11385" xr2:uid="{2E7DF291-7C4E-4872-AD47-758FC9565D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Freq</t>
   </si>
@@ -53,7 +53,10 @@
     <t>TIM1 (16-bit)</t>
   </si>
   <si>
-    <t>TIM0, TIM2 (8-bit)</t>
+    <t>TIM0 (8-bit)</t>
+  </si>
+  <si>
+    <t>TIM2 (8-bit)</t>
   </si>
 </sst>
 </file>
@@ -109,7 +112,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -285,22 +288,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
@@ -319,13 +338,150 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="15">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -360,8 +516,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC7CE"/>
       <color rgb="FF9C0006"/>
-      <color rgb="FFFFC7CE"/>
     </mruColors>
   </colors>
   <extLst>
@@ -373,6 +529,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>351626</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>9215</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31AEB1EC-2307-4F45-BF36-E253B06DDE47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="352425" y="4991100"/>
+          <a:ext cx="6390476" cy="2476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F692D45-E613-47B9-9051-4C0427654354}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333375" y="2533650"/>
+          <a:ext cx="6400000" cy="2409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>304000</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>47324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29F6422E-8A1E-4DA7-A788-B5D4FB5FA9FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="7572375"/>
+          <a:ext cx="6400000" cy="2409524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,30 +965,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32F2EC4-31DF-4C7E-8D03-F4E36AFF2780}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>6400</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -706,115 +999,158 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="12"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>6</v>
+      <c r="D5" s="19" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
-        <v>0</v>
-      </c>
-      <c r="B6" s="9">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <f>$B$2/($B$1*$A6)-1</f>
+        <v>39999</v>
+      </c>
+      <c r="C6" s="5">
+        <f>$B$2/($B$1*$A6)-1</f>
+        <v>39999</v>
+      </c>
+      <c r="D6" s="4">
         <f>$B$2/($B$1)-1</f>
-        <v>2499</v>
-      </c>
-      <c r="C6" s="7">
-        <f>$B$2/($B$1)-1</f>
-        <v>2499</v>
+        <v>39999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
         <v>8</v>
       </c>
-      <c r="B7" s="10">
-        <f t="shared" ref="B7:B11" si="0">$B$2/($B$1*A7)-1</f>
+      <c r="B7" s="6">
+        <f t="shared" ref="B7:C12" si="0">$B$2/($B$1*$A7)-1</f>
+        <v>4999</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>4999</v>
+      </c>
+      <c r="D7" s="3">
+        <f>$B$2/($B$1*A7)-1</f>
+        <v>4999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>32</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="3">
+        <f>$B$2/($B$1*A8)-1</f>
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>64</v>
+      </c>
+      <c r="B9" s="6">
+        <f t="shared" si="0"/>
+        <v>624</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
+        <v>624</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ref="D9:D12" si="1">$B$2/($B$1*A9)-1</f>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>128</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="3">
+        <f t="shared" si="1"/>
         <v>311.5</v>
       </c>
-      <c r="C7" s="3">
-        <f>$B$2/($B$1*A7)-1</f>
-        <v>311.5</v>
-      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>32</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="3">
-        <f>$B$2/($B$1*A8)-1</f>
-        <v>77.125</v>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>256</v>
+      </c>
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>155.25</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
+        <v>155.25</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>155.25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
-        <v>64</v>
-      </c>
-      <c r="B9" s="10">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>1024</v>
+      </c>
+      <c r="B12" s="8">
         <f t="shared" si="0"/>
         <v>38.0625</v>
       </c>
-      <c r="C9" s="3">
-        <f t="shared" ref="C9" si="1">$B$2/($B$1*A9)-1</f>
+      <c r="C12" s="8">
+        <f t="shared" si="0"/>
         <v>38.0625</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
-        <v>256</v>
-      </c>
-      <c r="B10" s="10">
-        <f t="shared" si="0"/>
-        <v>8.765625</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>1024</v>
-      </c>
-      <c r="B11" s="12">
-        <f t="shared" si="0"/>
-        <v>1.44140625</v>
-      </c>
-      <c r="C11" s="5"/>
+      <c r="D12" s="16">
+        <f t="shared" si="1"/>
+        <v>38.0625</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="A4:A5"/>
   </mergeCells>
-  <conditionalFormatting sqref="B6:B11">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="C6:C12">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>65535</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>255</formula>
+  <conditionalFormatting sqref="B6:D12">
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>MOD(B6,1)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:C11">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>MOD(B6,1)&gt;0</formula>
+  <conditionalFormatting sqref="B6:B12 D6:D12">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
+      <formula>255</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>